<commit_message>
work related to better cuts selection
</commit_message>
<xml_diff>
--- a/June2017/Runs_summary.xlsx
+++ b/June2017/Runs_summary.xlsx
@@ -16,18 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>[1-1 0]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>J0-2</t>
   </si>
   <si>
     <t>J0-4</t>
-  </si>
-  <si>
-    <t>[1 1 0]</t>
   </si>
   <si>
     <t>J0-3</t>
@@ -107,8 +101,33 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">E200: 
+    <t>[1-1 0]  &lt;100&gt; fitting single direction:</t>
+  </si>
+  <si>
+    <t>Ei400
+J0: 62.344 +/- 0.754; 
+J1: -5.894 +/- 0.854;
+J2: -7.533 +/- 0.216</t>
+  </si>
+  <si>
+    <t>J0: 32.772 +/- 0.284; [1,0,0]
+J0: 31.538 +/- 0.314; [0,1,0]
+J0: 34.208 +/- 0.272   [0,0,1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E200 NoA: 
+J0: 28.146 +/- 0.068;
+J1: 12.931 +/- 0.064;
+J2: -4.232 +/- 0.020 
+Ei400
+J0: 91.488 +/- 2.931; 
+J1: -11.325 +/- 2.388;
+J2: -15.305 +/- 0.563
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">E200 OldA: 
 J0: 32.831 +/- 4.352; J1: 14.463 +/- 4.168;
 J2: -0.422 +/- 1.429; J3: -1.871 +/- 0.475;
 J4: -0.960 +/- 0.715
@@ -140,16 +159,8 @@
     </r>
   </si>
   <si>
-    <t>Ei400-Fit J selected data isiscompute</t>
-  </si>
-  <si>
-    <t>E200
-Ei400
-J0: 34.554 +/- 0.057</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">E200: 
+    <r>
+      <t xml:space="preserve">E200 OldA
 J0: 28.917 +/- 0.038; J1: 20.613 +/- 0.029;
 J2: -1.147 +/- 0.003; J3: -2.028 +/- 0.002;
 E400noRl 
@@ -166,44 +177,82 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-</t>
+E400 -- changes due to </t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">alignment: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <color rgb="FFFE02C8"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>E400 -- look @ alignment: isiscomp-running</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">E200: 
-J0: 28.146 +/- 0.068;
-J1: 12.931 +/- 0.064;
-J2: -4.232 +/- 0.020 
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FFFE02C8"/>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Ei400 Fit J selected data PC W4</t>
-    </r>
+      <t xml:space="preserve"> J0: 41.226 +/- 2.001; J1: 19.442 +/- 1.589;
+ J2:  3.460 +/- 0.682;  J3: -5.047 +/- 0.239  </t>
+    </r>
+  </si>
+  <si>
+    <t>J0-1</t>
+  </si>
+  <si>
+    <t>E200
+Ei400 DS3
+ J0: 33.994 +/- 0.078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1 1 0]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1-1 0]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E200
+Ei400 DS3
+ J0: 33.72 +/- 0.1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+E400 DS3
+J0:26.497 +/- 0.496; 
+J1:  7.178 +/- 0.495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+E400 DS3
+J0: 25.6 +/- 0.8
+J1: 8.04+/- 0.8;
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,8 +282,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FFFE02C8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -260,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -272,9 +335,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -583,166 +643,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" customWidth="1"/>
-    <col min="6" max="6" width="48.42578125" customWidth="1"/>
+    <col min="1" max="2" width="34" customWidth="1"/>
+    <col min="3" max="4" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" customWidth="1"/>
+    <col min="7" max="7" width="48.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" ht="175.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="F4" s="2"/>
+      <c r="G4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
enhanced inputs for plot_Cuts.m plot_EnCuts.m and plot_dirCut.m and minor changes reflecting the current state of analysis.
</commit_message>
<xml_diff>
--- a/June2017/Runs_summary.xlsx
+++ b/June2017/Runs_summary.xlsx
@@ -104,26 +104,9 @@
     <t>[1-1 0]  &lt;100&gt; fitting single direction:</t>
   </si>
   <si>
-    <t>Ei400
-J0: 62.344 +/- 0.754; 
-J1: -5.894 +/- 0.854;
-J2: -7.533 +/- 0.216</t>
-  </si>
-  <si>
     <t>J0: 32.772 +/- 0.284; [1,0,0]
 J0: 31.538 +/- 0.314; [0,1,0]
 J0: 34.208 +/- 0.272   [0,0,1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E200 NoA: 
-J0: 28.146 +/- 0.068;
-J1: 12.931 +/- 0.064;
-J2: -4.232 +/- 0.020 
-Ei400
-J0: 91.488 +/- 2.931; 
-J1: -11.325 +/- 2.388;
-J2: -15.305 +/- 0.563
-</t>
   </si>
   <si>
     <r>
@@ -229,23 +212,70 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">E200
-Ei400 DS3
- J0: 33.72 +/- 0.1
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-E400 DS3
-J0:26.497 +/- 0.496; 
-J1:  7.178 +/- 0.495</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 E400 DS3
 J0: 25.6 +/- 0.8
 J1: 8.04+/- 0.8;
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+E400 DS3
+J0: 27.346 +/- 0.630
+J1:  6.549 +/- 0.626;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">E200 DS_enhanced 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J0: (running)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Ei400 DS3
+ J0: 33.72 +/- 0.1
+</t>
+    </r>
+  </si>
+  <si>
+    <t>E200 NoA: 
+J0: 28.146 +/- 0.068;
+J1: 12.931 +/- 0.064;
+J2: -4.232 +/- 0.020 
+Ei400 DS2
+J0: 91.488 +/- 2.931; 
+J1: -11.325 +/- 2.388;
+J2: -15.305 +/- 0.563
+E400 DS3
+J0:64.120 +/- 3.159; 
+J1: -8.249 +/- 2.186;
+J2: -7.536 +/- 0.524</t>
+  </si>
+  <si>
+    <t>Ei400
+J0: 62.344 +/- 0.754; 
+J1: -5.894 +/- 0.854;
+J2: -7.533 +/- 0.216
+Ei400 DS3
+J0: 65.663 +/- 3.055; 
+J1: -7.930 +/- 2.153; 
+J2: -8.047 +/- 0.476;</t>
   </si>
 </sst>
 </file>
@@ -646,7 +676,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +697,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>0</v>
@@ -679,43 +709,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="210" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="175.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>11</v>
@@ -755,7 +785,7 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>

</xml_diff>

<commit_message>
better interface for cut routines
Former-commit-id: ac4a2e10910051c83241696a9fc3cd69b10e5eab
</commit_message>
<xml_diff>
--- a/June2017/Runs_summary.xlsx
+++ b/June2017/Runs_summary.xlsx
@@ -225,6 +225,16 @@
 J1:  6.549 +/- 0.626;</t>
   </si>
   <si>
+    <t>Ei400
+J0: 62.344 +/- 0.754; 
+J1: -5.894 +/- 0.854;
+J2: -7.533 +/- 0.216
+Ei400 DS3
+J0: 65.663 +/- 3.055; 
+J1: -7.930 +/- 2.153; 
+J2: -8.047 +/- 0.476;</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">E200 DS_enhanced 
 </t>
@@ -232,12 +242,11 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF00B050"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>J0: (running)</t>
+      <t>J0: 27.8836 +/- 0.08</t>
     </r>
     <r>
       <rPr>
@@ -254,7 +263,7 @@
     </r>
   </si>
   <si>
-    <t>E200 NoA: 
+    <t>E200: 
 J0: 28.146 +/- 0.068;
 J1: 12.931 +/- 0.064;
 J2: -4.232 +/- 0.020 
@@ -267,22 +276,12 @@
 J1: -8.249 +/- 2.186;
 J2: -7.536 +/- 0.524</t>
   </si>
-  <si>
-    <t>Ei400
-J0: 62.344 +/- 0.754; 
-J1: -5.894 +/- 0.854;
-J2: -7.533 +/- 0.216
-Ei400 DS3
-J0: 65.663 +/- 3.055; 
-J1: -7.930 +/- 2.153; 
-J2: -8.047 +/- 0.476;</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,6 +327,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -676,7 +681,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,13 +720,13 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
@@ -742,7 +747,7 @@
         <v>21</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>15</v>

</xml_diff>